<commit_message>
Changes related to excel output
</commit_message>
<xml_diff>
--- a/asx_1.xlsx
+++ b/asx_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\personal_project\ASX-dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/storezadeveloper/Projects/ComparisonTrade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96388C21-5C87-4BF6-829F-BE4C376FDAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DB9A1-ACD1-3043-8F9D-D27ABA737AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,27 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
-    <t xml:space="preserve">Stock Code </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Company Name        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sector          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Open    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Close   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Volume    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trade Date  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Market Cap</t>
   </si>
   <si>
@@ -115,6 +94,27 @@
   </si>
   <si>
     <t xml:space="preserve"> 82.1B</t>
+  </si>
+  <si>
+    <t>Stock Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trade Date</t>
   </si>
 </sst>
 </file>
@@ -435,51 +435,51 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2">
         <v>45.2</v>
@@ -491,21 +491,21 @@
         <v>2500000</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>102.5</v>
@@ -517,21 +517,21 @@
         <v>1850000</v>
       </c>
       <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>24.3</v>
@@ -543,21 +543,21 @@
         <v>1200000</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>291.39999999999998</v>
@@ -569,21 +569,21 @@
         <v>455000</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>127.8</v>
@@ -595,21 +595,21 @@
         <v>680000</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>28.9</v>
@@ -621,10 +621,10 @@
         <v>950000</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel showing Tolerance based category
</commit_message>
<xml_diff>
--- a/asx_1.xlsx
+++ b/asx_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/storezadeveloper/Projects/ComparisonTrade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DB9A1-ACD1-3043-8F9D-D27ABA737AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CF6D91-CFDC-FA41-987D-8C040972B9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
-  <si>
-    <t xml:space="preserve"> Market Cap</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">BHP       </t>
   </si>
@@ -42,9 +39,6 @@
     <t xml:space="preserve"> 2024-03-01 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 231.8B</t>
-  </si>
-  <si>
     <t xml:space="preserve">CBA       </t>
   </si>
   <si>
@@ -54,18 +48,12 @@
     <t xml:space="preserve"> Financials     </t>
   </si>
   <si>
-    <t xml:space="preserve"> 175.2B</t>
-  </si>
-  <si>
     <t xml:space="preserve">WBC       </t>
   </si>
   <si>
     <t xml:space="preserve"> Westpac Banking    </t>
   </si>
   <si>
-    <t xml:space="preserve"> 85.3B</t>
-  </si>
-  <si>
     <t xml:space="preserve">CSL       </t>
   </si>
   <si>
@@ -75,46 +63,40 @@
     <t xml:space="preserve"> Healthcare     </t>
   </si>
   <si>
-    <t xml:space="preserve"> 141.5B</t>
-  </si>
-  <si>
     <t xml:space="preserve">RIO       </t>
   </si>
   <si>
     <t xml:space="preserve"> Rio Tinto Limited  </t>
   </si>
   <si>
-    <t xml:space="preserve"> 47.2B</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANZ       </t>
   </si>
   <si>
     <t xml:space="preserve"> ANZ Banking Group  </t>
   </si>
   <si>
-    <t xml:space="preserve"> 82.1B</t>
-  </si>
-  <si>
     <t>Stock Code</t>
   </si>
   <si>
-    <t xml:space="preserve"> Company Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trade Date</t>
+    <t>Market Cap</t>
+  </si>
+  <si>
+    <t>Trade Date</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Company Name</t>
   </si>
 </sst>
 </file>
@@ -435,7 +417,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -447,39 +429,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
       <c r="D2">
         <v>45.2</v>
@@ -491,21 +473,21 @@
         <v>2500000</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>231.8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>102.5</v>
@@ -517,21 +499,21 @@
         <v>1850000</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>175.2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>24.3</v>
@@ -543,21 +525,21 @@
         <v>1200000</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>85.3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>291.39999999999998</v>
@@ -569,21 +551,21 @@
         <v>455000</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>141.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>127.8</v>
@@ -595,21 +577,21 @@
         <v>680000</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>47.2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>28.9</v>
@@ -621,10 +603,10 @@
         <v>950000</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>82.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Seconf rule check based on Threshold
</commit_message>
<xml_diff>
--- a/asx_1.xlsx
+++ b/asx_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/storezadeveloper/Projects/ComparisonTrade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CF6D91-CFDC-FA41-987D-8C040972B9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9F390-7B98-9345-A607-8E72315761F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t xml:space="preserve">BHP       </t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshi     </t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -425,6 +428,7 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,6 +613,32 @@
         <v>82.1</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>28.9</v>
+      </c>
+      <c r="E8">
+        <v>29.15</v>
+      </c>
+      <c r="F8">
+        <v>950000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>82.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Date and string comparison implemented but not generic
</commit_message>
<xml_diff>
--- a/asx_1.xlsx
+++ b/asx_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/storezadeveloper/Projects/ComparisonTrade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9F390-7B98-9345-A607-8E72315761F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892F3ED8-03B7-B946-9053-DB1F9CDD6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14200" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,64 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">BHP       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BHP Group Ltd      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Materials      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2024-03-01 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBA       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Commonwealth Bank  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Financials     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WBC       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Westpac Banking    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSL       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CSL Limited        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Healthcare     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIO       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rio Tinto Limited  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANZ       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ANZ Banking Group  </t>
-  </si>
-  <si>
-    <t>Stock Code</t>
-  </si>
-  <si>
-    <t>Market Cap</t>
-  </si>
-  <si>
-    <t>Trade Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Volume</t>
   </si>
@@ -96,10 +39,64 @@
     <t>Sector</t>
   </si>
   <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshi     </t>
+    <t>BHP</t>
+  </si>
+  <si>
+    <t>CBA</t>
+  </si>
+  <si>
+    <t>WBC</t>
+  </si>
+  <si>
+    <t>CSL</t>
+  </si>
+  <si>
+    <t>StockCode</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>TradeDate</t>
+  </si>
+  <si>
+    <t>MarketCap</t>
+  </si>
+  <si>
+    <t>BHPGroupLtd</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>CommonwealthBank</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>WestpacBanking</t>
+  </si>
+  <si>
+    <t>CSLLimited</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>RIO</t>
+  </si>
+  <si>
+    <t>RioTintoLimited</t>
+  </si>
+  <si>
+    <t>ANZ</t>
+  </si>
+  <si>
+    <t>ANZBankingGroup</t>
+  </si>
+  <si>
+    <t>Joshi</t>
   </si>
 </sst>
 </file>
@@ -135,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +418,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -433,39 +431,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>45.2</v>
@@ -476,8 +474,8 @@
       <c r="F2">
         <v>2500000</v>
       </c>
-      <c r="G2" t="s">
-        <v>3</v>
+      <c r="G2" s="1">
+        <v>45352</v>
       </c>
       <c r="H2">
         <v>231.8</v>
@@ -485,13 +483,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>102.5</v>
@@ -502,8 +500,8 @@
       <c r="F3">
         <v>1850000</v>
       </c>
-      <c r="G3" t="s">
-        <v>3</v>
+      <c r="G3" s="1">
+        <v>45352</v>
       </c>
       <c r="H3">
         <v>175.2</v>
@@ -511,13 +509,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>24.3</v>
@@ -528,8 +526,8 @@
       <c r="F4">
         <v>1200000</v>
       </c>
-      <c r="G4" t="s">
-        <v>3</v>
+      <c r="G4" s="1">
+        <v>45352</v>
       </c>
       <c r="H4">
         <v>85.3</v>
@@ -537,13 +535,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>291.39999999999998</v>
@@ -554,8 +552,8 @@
       <c r="F5">
         <v>455000</v>
       </c>
-      <c r="G5" t="s">
-        <v>3</v>
+      <c r="G5" s="1">
+        <v>45352</v>
       </c>
       <c r="H5">
         <v>141.5</v>
@@ -563,13 +561,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
       </c>
       <c r="D6">
         <v>127.8</v>
@@ -580,8 +578,8 @@
       <c r="F6">
         <v>680000</v>
       </c>
-      <c r="G6" t="s">
-        <v>3</v>
+      <c r="G6" s="1">
+        <v>45352</v>
       </c>
       <c r="H6">
         <v>47.2</v>
@@ -589,13 +587,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
       <c r="D7">
         <v>28.9</v>
@@ -606,8 +604,8 @@
       <c r="F7">
         <v>950000</v>
       </c>
-      <c r="G7" t="s">
-        <v>3</v>
+      <c r="G7" s="1">
+        <v>45352</v>
       </c>
       <c r="H7">
         <v>82.1</v>
@@ -615,13 +613,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
       </c>
       <c r="D8">
         <v>28.9</v>
@@ -632,8 +630,8 @@
       <c r="F8">
         <v>950000</v>
       </c>
-      <c r="G8" t="s">
-        <v>3</v>
+      <c r="G8" s="1">
+        <v>45352</v>
       </c>
       <c r="H8">
         <v>82.1</v>

</xml_diff>